<commit_message>
NPV Cash Flow Model
</commit_message>
<xml_diff>
--- a/TESLA HISTORIC ANALYSIS.xlsx
+++ b/TESLA HISTORIC ANALYSIS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/396cb21c71a230ab/Área de Trabalho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2501" documentId="11_AD4DF034E34935FBC521DC2C77996C245ADEDD8E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{030C1F03-C410-4F36-9544-3CB9A29F18B9}"/>
+  <xr:revisionPtr revIDLastSave="2530" documentId="11_AD4DF034E34935FBC521DC2C77996C245ADEDD8E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7A1D776B-BEA7-4610-B5BC-56EC577420CB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="209">
   <si>
     <t>Assets</t>
   </si>
@@ -664,6 +664,9 @@
   </si>
   <si>
     <t>Accounts Payable Ratio</t>
+  </si>
+  <si>
+    <t>Research and development</t>
   </si>
 </sst>
 </file>
@@ -684,7 +687,7 @@
     <numFmt numFmtId="173" formatCode="0.00%;[Red]\(0.00%\);\-"/>
     <numFmt numFmtId="174" formatCode="#,##0.00;[Red]\(#,##0.00\);\-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,6 +766,14 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -790,7 +801,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -887,6 +898,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -894,7 +916,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -992,15 +1014,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="172" fontId="7" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1045,12 +1058,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1102,6 +1109,30 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2419,11 +2450,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15.95" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2434,25 +2465,25 @@
     <col min="13" max="16384" width="15.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>2010</v>
       </c>
@@ -2487,7 +2518,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +2531,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
@@ -2516,7 +2547,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -2554,7 +2585,7 @@
         <v>19384000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>112</v>
       </c>
@@ -2592,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -2629,8 +2660,9 @@
       <c r="L10" s="5">
         <v>1886000</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="70"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -2668,7 +2700,7 @@
         <v>4101000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -2706,7 +2738,7 @@
         <v>1346000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="8" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
@@ -2755,7 +2787,7 @@
         <v>26717000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2768,7 +2800,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -2806,7 +2838,7 @@
         <v>3091000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -4301,43 +4333,43 @@
         <v>33</v>
       </c>
       <c r="B61" s="9">
-        <f t="shared" ref="B61:K61" si="7">+SUM(B55:B60)</f>
+        <f>+SUM(B55:B60)</f>
         <v>207048</v>
       </c>
       <c r="C61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(C55:C60)</f>
         <v>224045</v>
       </c>
       <c r="D61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(D55:D60)</f>
         <v>124700</v>
       </c>
       <c r="E61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(E55:E60)</f>
         <v>667120</v>
       </c>
       <c r="F61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(F55:F60)</f>
         <v>911710</v>
       </c>
       <c r="G61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(G55:G60)</f>
         <v>1088944</v>
       </c>
       <c r="H61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(H55:H60)</f>
         <v>4752911</v>
       </c>
       <c r="I61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(I55:I60)</f>
         <v>4237242</v>
       </c>
       <c r="J61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(J55:J60)</f>
         <v>4923000</v>
       </c>
       <c r="K61" s="9">
-        <f t="shared" si="7"/>
+        <f>+SUM(K55:K60)</f>
         <v>6619000</v>
       </c>
       <c r="L61" s="9">
@@ -4482,11 +4514,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D81EB9-6E77-48CA-9D7D-5C7277E9620B}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15.95" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5179,7 +5211,7 @@
     </row>
     <row r="24" spans="1:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>208</v>
       </c>
       <c r="B24" s="5">
         <v>19282</v>
@@ -6004,18 +6036,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA2F769-4A7F-4E0C-845A-BCDD874B6CEE}">
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" style="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" style="1" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" style="5" customWidth="1" outlineLevel="1"/>
     <col min="9" max="13" width="15.7109375" style="5"/>
     <col min="14" max="16384" width="15.7109375" style="1"/>
@@ -6083,8 +6115,8 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:13" s="8" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="71" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="9"/>
@@ -7127,8 +7159,8 @@
       <c r="L38" s="14"/>
       <c r="M38" s="14"/>
     </row>
-    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+    <row r="39" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="71" t="s">
         <v>75</v>
       </c>
       <c r="B39" s="14"/>
@@ -7490,8 +7522,8 @@
       <c r="L52" s="14"/>
       <c r="M52" s="14"/>
     </row>
-    <row r="53" spans="1:13" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+    <row r="53" spans="1:13" s="8" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="71" t="s">
         <v>83</v>
       </c>
       <c r="B53" s="14"/>
@@ -7819,61 +7851,88 @@
       <c r="M62" s="14"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="B63" s="14">
+      <c r="B63" s="28">
         <v>-2046</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C63" s="28">
         <v>-3734</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E63" s="14">
+      <c r="E63" s="28">
         <v>188796</v>
       </c>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14">
+      <c r="F63" s="28"/>
+      <c r="G63" s="28">
         <v>3271</v>
       </c>
-      <c r="H63" s="14">
+      <c r="H63" s="28">
         <v>568745</v>
       </c>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14">
+      <c r="I63" s="28"/>
+      <c r="J63" s="28">
         <v>287213</v>
       </c>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14">
+      <c r="K63" s="28"/>
+      <c r="L63" s="28">
         <v>174000</v>
       </c>
-      <c r="M63" s="14"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14">
-        <v>52883</v>
-      </c>
-      <c r="K64" s="14">
-        <v>437000</v>
-      </c>
-      <c r="L64" s="14">
-        <v>279000</v>
-      </c>
-      <c r="M64" s="14">
-        <v>24000</v>
+      <c r="M63" s="28"/>
+    </row>
+    <row r="64" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="16">
+        <f>+SUM(B54:B63)</f>
+        <v>155419</v>
+      </c>
+      <c r="C64" s="16">
+        <f>+SUM(C54:C63)</f>
+        <v>338045</v>
+      </c>
+      <c r="D64" s="16">
+        <f>+SUM(D54:D63)</f>
+        <v>446000</v>
+      </c>
+      <c r="E64" s="16">
+        <f>+SUM(E54:E63)</f>
+        <v>419635</v>
+      </c>
+      <c r="F64" s="16">
+        <f>+SUM(F54:F63)</f>
+        <v>635422</v>
+      </c>
+      <c r="G64" s="16">
+        <f>+SUM(G54:G63)</f>
+        <v>2143130</v>
+      </c>
+      <c r="H64" s="16">
+        <f>+SUM(H54:H63)</f>
+        <v>1523523</v>
+      </c>
+      <c r="I64" s="16">
+        <v>3743976</v>
+      </c>
+      <c r="J64" s="16">
+        <v>4414864</v>
+      </c>
+      <c r="K64" s="16">
+        <v>574000</v>
+      </c>
+      <c r="L64" s="16">
+        <v>1529000</v>
+      </c>
+      <c r="M64" s="16">
+        <v>9973000</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="6"/>
       <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
@@ -7883,55 +7942,91 @@
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
-      <c r="K65" s="14">
-        <v>-227000</v>
-      </c>
-      <c r="L65" s="14">
-        <v>-311000</v>
-      </c>
-      <c r="M65" s="14">
-        <v>-208000</v>
-      </c>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14">
-        <v>-230385</v>
-      </c>
-      <c r="K66" s="14">
-        <v>-6000</v>
-      </c>
-      <c r="L66" s="14">
-        <v>-9000</v>
-      </c>
-      <c r="M66" s="14">
-        <v>-35000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14">
-        <v>201527</v>
-      </c>
-      <c r="J67" s="14">
-        <v>789704</v>
-      </c>
-      <c r="K67" s="14"/>
-      <c r="L67" s="14"/>
-      <c r="M67" s="14"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28">
+        <v>-35525</v>
+      </c>
+      <c r="H66" s="28">
+        <v>-34278</v>
+      </c>
+      <c r="I66" s="28">
+        <v>-6553</v>
+      </c>
+      <c r="J66" s="28">
+        <v>39726</v>
+      </c>
+      <c r="K66" s="28">
+        <v>-23000</v>
+      </c>
+      <c r="L66" s="28">
+        <v>8000</v>
+      </c>
+      <c r="M66" s="28">
+        <v>334000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" s="8" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="16">
+        <f>+B64+B51+B37</f>
+        <v>60350</v>
+      </c>
+      <c r="C67" s="16">
+        <f>+C64+C51+C37</f>
+        <v>29931</v>
+      </c>
+      <c r="D67" s="16">
+        <f>+D64+D51+D37</f>
+        <v>155707</v>
+      </c>
+      <c r="E67" s="16">
+        <f>+E64+E51+E37</f>
+        <v>-53376</v>
+      </c>
+      <c r="F67" s="16">
+        <f>+F64+F51+F37</f>
+        <v>643999</v>
+      </c>
+      <c r="G67" s="16">
+        <f>+G64+G51+G37+G66</f>
+        <v>1059824</v>
+      </c>
+      <c r="H67" s="16">
+        <f>+H64+H51+H37+H66</f>
+        <v>-708805</v>
+      </c>
+      <c r="I67" s="16">
+        <f>+I64+I51+I37+I66</f>
+        <v>2532509</v>
+      </c>
+      <c r="J67" s="16">
+        <f>+J64+J51+J37+J66</f>
+        <v>198059</v>
+      </c>
+      <c r="K67" s="16">
+        <f>+K64+K51+K37+K66</f>
+        <v>312000</v>
+      </c>
+      <c r="L67" s="16">
+        <f>+L64+L51+L37+L66</f>
+        <v>2506000</v>
+      </c>
+      <c r="M67" s="16">
+        <f>+M64+M51+M37+M66</f>
+        <v>13118000</v>
+      </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B68" s="14"/>
@@ -7941,88 +8036,117 @@
       <c r="F68" s="14"/>
       <c r="G68" s="14"/>
       <c r="H68" s="14"/>
-      <c r="I68" s="14">
-        <v>-21250</v>
-      </c>
-      <c r="J68" s="14">
-        <v>-261844</v>
-      </c>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
       <c r="K68" s="14"/>
       <c r="L68" s="14"/>
       <c r="M68" s="14"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="26"/>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28">
-        <v>-373</v>
-      </c>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="28"/>
-    </row>
-    <row r="70" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B70" s="16">
-        <f>+SUM(B54:B69)</f>
-        <v>155419</v>
-      </c>
-      <c r="C70" s="16">
-        <f t="shared" ref="C70:D70" si="17">+SUM(C54:C69)</f>
-        <v>338045</v>
-      </c>
-      <c r="D70" s="16">
+      <c r="A69" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B69" s="14">
+        <v>9277</v>
+      </c>
+      <c r="C69" s="14">
+        <f t="shared" ref="C69:J69" si="17">+B70</f>
+        <v>69627</v>
+      </c>
+      <c r="D69" s="14">
         <f t="shared" si="17"/>
-        <v>446000</v>
-      </c>
-      <c r="E70" s="16">
-        <f t="shared" ref="E70" si="18">+SUM(E54:E69)</f>
-        <v>419635</v>
-      </c>
-      <c r="F70" s="16">
-        <f t="shared" ref="F70" si="19">+SUM(F54:F69)</f>
-        <v>635422</v>
-      </c>
-      <c r="G70" s="16">
-        <f t="shared" ref="G70" si="20">+SUM(G54:G69)</f>
-        <v>2143130</v>
-      </c>
-      <c r="H70" s="16">
-        <f t="shared" ref="H70" si="21">+SUM(H54:H69)</f>
-        <v>1523523</v>
-      </c>
-      <c r="I70" s="16">
-        <f t="shared" ref="I70" si="22">+SUM(I54:I69)</f>
-        <v>3743976</v>
-      </c>
-      <c r="J70" s="16">
-        <f t="shared" ref="J70" si="23">+SUM(J54:J69)</f>
-        <v>4414864</v>
-      </c>
-      <c r="K70" s="16">
-        <f t="shared" ref="K70" si="24">+SUM(K54:K69)</f>
-        <v>574000</v>
-      </c>
-      <c r="L70" s="16">
-        <f t="shared" ref="L70" si="25">+SUM(L54:L69)</f>
-        <v>1529000</v>
-      </c>
-      <c r="M70" s="16">
-        <f t="shared" ref="M70" si="26">+SUM(M54:M69)</f>
-        <v>9973000</v>
+        <v>99558</v>
+      </c>
+      <c r="E69" s="14">
+        <f t="shared" si="17"/>
+        <v>255265</v>
+      </c>
+      <c r="F69" s="14">
+        <f t="shared" si="17"/>
+        <v>201889</v>
+      </c>
+      <c r="G69" s="14">
+        <f t="shared" si="17"/>
+        <v>845888</v>
+      </c>
+      <c r="H69" s="14">
+        <f t="shared" si="17"/>
+        <v>1905712</v>
+      </c>
+      <c r="I69" s="14">
+        <f t="shared" si="17"/>
+        <v>1196907</v>
+      </c>
+      <c r="J69" s="14">
+        <f t="shared" si="17"/>
+        <v>3729416</v>
+      </c>
+      <c r="K69" s="14">
+        <v>3965000</v>
+      </c>
+      <c r="L69" s="14">
+        <f t="shared" ref="L69:M69" si="18">+K70</f>
+        <v>4277000</v>
+      </c>
+      <c r="M69" s="14">
+        <f t="shared" si="18"/>
+        <v>6783000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B70" s="14">
+        <f t="shared" ref="B70:K70" si="19">+B69+B67</f>
+        <v>69627</v>
+      </c>
+      <c r="C70" s="14">
+        <f t="shared" si="19"/>
+        <v>99558</v>
+      </c>
+      <c r="D70" s="14">
+        <f t="shared" si="19"/>
+        <v>255265</v>
+      </c>
+      <c r="E70" s="14">
+        <f t="shared" si="19"/>
+        <v>201889</v>
+      </c>
+      <c r="F70" s="14">
+        <f t="shared" si="19"/>
+        <v>845888</v>
+      </c>
+      <c r="G70" s="14">
+        <f t="shared" si="19"/>
+        <v>1905712</v>
+      </c>
+      <c r="H70" s="14">
+        <f t="shared" si="19"/>
+        <v>1196907</v>
+      </c>
+      <c r="I70" s="14">
+        <f t="shared" si="19"/>
+        <v>3729416</v>
+      </c>
+      <c r="J70" s="14">
+        <f t="shared" si="19"/>
+        <v>3927475</v>
+      </c>
+      <c r="K70" s="14">
+        <f t="shared" si="19"/>
+        <v>4277000</v>
+      </c>
+      <c r="L70" s="14">
+        <f t="shared" ref="L70:M70" si="20">+L69+L67</f>
+        <v>6783000</v>
+      </c>
+      <c r="M70" s="14">
+        <f t="shared" si="20"/>
+        <v>19901000</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="6"/>
       <c r="B71" s="14"/>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
@@ -8036,323 +8160,283 @@
       <c r="L71" s="14"/>
       <c r="M71" s="14"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="26"/>
-      <c r="B72" s="28"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="28">
-        <v>-35525</v>
-      </c>
-      <c r="H72" s="28">
-        <v>-34278</v>
-      </c>
-      <c r="I72" s="28">
-        <v>-6553</v>
-      </c>
-      <c r="J72" s="28">
-        <v>39726</v>
-      </c>
-      <c r="K72" s="28">
-        <v>-23000</v>
-      </c>
-      <c r="L72" s="28">
-        <v>8000</v>
-      </c>
-      <c r="M72" s="28">
-        <v>334000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B73" s="16">
-        <f>+B70+B51+B37</f>
-        <v>60350</v>
-      </c>
-      <c r="C73" s="16">
-        <f t="shared" ref="C73:F73" si="27">+C70+C51+C37</f>
-        <v>29931</v>
-      </c>
-      <c r="D73" s="16">
-        <f t="shared" si="27"/>
-        <v>155707</v>
-      </c>
-      <c r="E73" s="16">
-        <f>+E70+E51+E37</f>
-        <v>-53376</v>
-      </c>
-      <c r="F73" s="16">
-        <f t="shared" si="27"/>
-        <v>643999</v>
-      </c>
-      <c r="G73" s="16">
-        <f>+G70+G51+G37+G72</f>
-        <v>1059824</v>
-      </c>
-      <c r="H73" s="16">
-        <f>+H70+H51+H37+H72</f>
-        <v>-708805</v>
-      </c>
-      <c r="I73" s="16">
-        <f t="shared" ref="I73:J73" si="28">+I70+I51+I37+I72</f>
-        <v>2532509</v>
-      </c>
-      <c r="J73" s="16">
-        <f t="shared" si="28"/>
-        <v>198059</v>
-      </c>
-      <c r="K73" s="16">
-        <f t="shared" ref="K73" si="29">+K70+K51+K37+K72</f>
-        <v>312000</v>
-      </c>
-      <c r="L73" s="16">
-        <f t="shared" ref="L73" si="30">+L70+L51+L37+L72</f>
-        <v>2506000</v>
-      </c>
-      <c r="M73" s="16">
-        <f>+M70+M51+M37+M72</f>
-        <v>13118000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14"/>
-      <c r="L74" s="14"/>
-      <c r="M74" s="14"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B75" s="14">
-        <v>9277</v>
-      </c>
-      <c r="C75" s="14">
-        <f t="shared" ref="C75:J75" si="31">+B76</f>
-        <v>69627</v>
-      </c>
-      <c r="D75" s="14">
-        <f t="shared" si="31"/>
-        <v>99558</v>
-      </c>
-      <c r="E75" s="14">
-        <f t="shared" si="31"/>
-        <v>255265</v>
-      </c>
-      <c r="F75" s="14">
-        <f t="shared" si="31"/>
-        <v>201889</v>
-      </c>
-      <c r="G75" s="14">
-        <f t="shared" si="31"/>
-        <v>845888</v>
-      </c>
-      <c r="H75" s="14">
-        <f t="shared" si="31"/>
-        <v>1905712</v>
-      </c>
-      <c r="I75" s="14">
-        <f t="shared" si="31"/>
-        <v>1196907</v>
-      </c>
-      <c r="J75" s="14">
-        <f t="shared" si="31"/>
-        <v>3729416</v>
-      </c>
-      <c r="K75" s="14">
-        <v>3965000</v>
-      </c>
-      <c r="L75" s="14">
-        <f t="shared" ref="L75:M75" si="32">+K76</f>
-        <v>4277000</v>
-      </c>
-      <c r="M75" s="14">
-        <f t="shared" si="32"/>
-        <v>6783000</v>
-      </c>
+    <row r="72" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="16"/>
+      <c r="I72" s="16"/>
+      <c r="J72" s="16"/>
+      <c r="K72" s="16"/>
+      <c r="L72" s="16"/>
+      <c r="M72" s="16"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B73" s="14">
+        <v>70</v>
+      </c>
+      <c r="C73" s="14">
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="D73" s="14">
+        <v>3.472</v>
+      </c>
+      <c r="E73" s="14">
+        <v>6938</v>
+      </c>
+      <c r="F73" s="14">
+        <v>9041</v>
+      </c>
+      <c r="G73" s="14">
+        <v>20539</v>
+      </c>
+      <c r="H73" s="14">
+        <v>32060</v>
+      </c>
+      <c r="I73" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="J73" s="14">
+        <v>10.528</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="L73" s="14">
+        <v>207</v>
+      </c>
+      <c r="M73" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" s="14">
+        <v>171</v>
+      </c>
+      <c r="C74" s="14">
+        <v>9</v>
+      </c>
+      <c r="D74" s="14">
+        <v>282</v>
+      </c>
+      <c r="E74" s="14">
+        <v>117</v>
+      </c>
+      <c r="F74" s="14">
+        <v>257</v>
+      </c>
+      <c r="G74" s="14">
+        <v>3120</v>
+      </c>
+      <c r="H74" s="14">
+        <v>9461</v>
+      </c>
+      <c r="I74" s="14">
+        <v>663.77099999999996</v>
+      </c>
+      <c r="J74" s="14">
+        <v>914.10799999999995</v>
+      </c>
+      <c r="K74" s="14">
+        <v>249</v>
+      </c>
+      <c r="L74" s="14">
+        <v>562</v>
+      </c>
+      <c r="M74" s="14">
+        <v>1.0880000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B76" s="14">
-        <f t="shared" ref="B76:K76" si="33">+B75+B73</f>
-        <v>69627</v>
-      </c>
-      <c r="C76" s="14">
-        <f t="shared" si="33"/>
-        <v>99558</v>
-      </c>
-      <c r="D76" s="14">
-        <f t="shared" si="33"/>
-        <v>255265</v>
-      </c>
-      <c r="E76" s="14">
-        <f t="shared" si="33"/>
-        <v>201889</v>
-      </c>
-      <c r="F76" s="14">
-        <f t="shared" si="33"/>
-        <v>845888</v>
-      </c>
-      <c r="G76" s="14">
-        <f t="shared" si="33"/>
-        <v>1905712</v>
-      </c>
-      <c r="H76" s="14">
-        <f t="shared" si="33"/>
-        <v>1196907</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
       <c r="I76" s="14">
-        <f t="shared" si="33"/>
-        <v>3729416</v>
+        <v>307.87900000000002</v>
       </c>
       <c r="J76" s="14">
-        <f t="shared" si="33"/>
-        <v>3927475</v>
+        <v>313.483</v>
       </c>
       <c r="K76" s="14">
-        <f t="shared" si="33"/>
-        <v>4277000</v>
-      </c>
-      <c r="L76" s="14">
-        <f t="shared" ref="L76:M76" si="34">+L75+L73</f>
-        <v>6783000</v>
-      </c>
-      <c r="M76" s="14">
-        <f t="shared" si="34"/>
-        <v>19901000</v>
+        <v>94</v>
+      </c>
+      <c r="L76" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="M76" s="14" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
+      <c r="A77" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="14">
+        <v>319.22500000000002</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="14">
+        <v>44.89</v>
+      </c>
+      <c r="F77" s="14">
+        <v>38.789000000000001</v>
+      </c>
+      <c r="G77" s="14">
+        <v>254.393</v>
+      </c>
+      <c r="H77" s="14">
+        <v>267.334</v>
+      </c>
       <c r="I77" s="14"/>
       <c r="J77" s="14"/>
       <c r="K77" s="14"/>
       <c r="L77" s="14"/>
       <c r="M77" s="14"/>
     </row>
-    <row r="78" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="16"/>
-      <c r="H78" s="16"/>
-      <c r="I78" s="16"/>
-      <c r="J78" s="16"/>
-      <c r="K78" s="16"/>
-      <c r="L78" s="16"/>
-      <c r="M78" s="16"/>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="14">
+        <v>6.9619999999999997</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14">
+        <v>38.692999999999998</v>
+      </c>
+      <c r="J78" s="14">
+        <v>182.571</v>
+      </c>
+      <c r="K78" s="14">
+        <v>381</v>
+      </c>
+      <c r="L78" s="14">
+        <v>455</v>
+      </c>
+      <c r="M78" s="14">
+        <v>444</v>
+      </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B79" s="14">
-        <v>70</v>
+        <v>103</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C79" s="14">
-        <v>1.1379999999999999</v>
-      </c>
-      <c r="D79" s="14">
-        <v>3.472</v>
-      </c>
-      <c r="E79" s="14">
-        <v>6938</v>
-      </c>
-      <c r="F79" s="14">
-        <v>9041</v>
-      </c>
+        <v>6.2939999999999996</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
       <c r="G79" s="14">
-        <v>20539</v>
+        <v>50.076000000000001</v>
       </c>
       <c r="H79" s="14">
-        <v>32060</v>
-      </c>
-      <c r="I79" s="14" t="s">
-        <v>148</v>
+        <v>174.749</v>
+      </c>
+      <c r="I79" s="14">
+        <v>16.385000000000002</v>
       </c>
       <c r="J79" s="14">
-        <v>10.528</v>
-      </c>
-      <c r="K79" s="14" t="s">
-        <v>114</v>
+        <v>65.694999999999993</v>
+      </c>
+      <c r="K79" s="14">
+        <v>35</v>
       </c>
       <c r="L79" s="14">
-        <v>207</v>
-      </c>
-      <c r="M79" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="M79" s="14">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B80" s="14">
-        <v>171</v>
+        <v>104</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C80" s="14">
-        <v>9</v>
-      </c>
-      <c r="D80" s="14">
-        <v>282</v>
-      </c>
-      <c r="E80" s="14">
-        <v>117</v>
-      </c>
-      <c r="F80" s="14">
-        <v>257</v>
-      </c>
-      <c r="G80" s="14">
-        <v>3120</v>
-      </c>
-      <c r="H80" s="14">
-        <v>9461</v>
-      </c>
-      <c r="I80" s="14">
-        <v>663.77099999999996</v>
-      </c>
-      <c r="J80" s="14">
-        <v>914.10799999999995</v>
-      </c>
-      <c r="K80" s="14">
-        <v>249</v>
-      </c>
-      <c r="L80" s="14">
-        <v>562</v>
-      </c>
-      <c r="M80" s="14">
-        <v>1.0880000000000001</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B81" s="14">
+        <v>86.224999999999994</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>3</v>
+      </c>
       <c r="E81" s="14"/>
       <c r="F81" s="14"/>
       <c r="G81" s="14"/>
@@ -8365,56 +8449,44 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
+        <v>106</v>
+      </c>
+      <c r="B82" s="14">
+        <v>19.073</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>3</v>
+      </c>
       <c r="E82" s="14"/>
       <c r="F82" s="14"/>
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
-      <c r="I82" s="14">
-        <v>307.87900000000002</v>
-      </c>
-      <c r="J82" s="14">
-        <v>313.483</v>
-      </c>
-      <c r="K82" s="14">
-        <v>94</v>
-      </c>
-      <c r="L82" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="M82" s="14" t="s">
-        <v>114</v>
-      </c>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B83" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B83" s="14">
+        <v>1.7909999999999999</v>
+      </c>
+      <c r="C83" s="14" t="s">
         <v>3</v>
-      </c>
-      <c r="C83" s="14">
-        <v>319.22500000000002</v>
       </c>
       <c r="D83" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E83" s="14">
-        <v>44.89</v>
-      </c>
-      <c r="F83" s="14">
-        <v>38.789000000000001</v>
-      </c>
-      <c r="G83" s="14">
-        <v>254.393</v>
-      </c>
-      <c r="H83" s="14">
-        <v>267.334</v>
-      </c>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
       <c r="K83" s="14"/>
@@ -8423,87 +8495,45 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>3</v>
+        <v>108</v>
+      </c>
+      <c r="B84" s="14">
+        <v>183</v>
       </c>
       <c r="C84" s="14">
-        <v>6.9619999999999997</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>3</v>
+        <v>4.4820000000000002</v>
+      </c>
+      <c r="D84" s="14">
+        <v>2.7029999999999998</v>
       </c>
       <c r="E84" s="14"/>
       <c r="F84" s="14"/>
       <c r="G84" s="14"/>
       <c r="H84" s="14"/>
-      <c r="I84" s="14">
-        <v>38.692999999999998</v>
-      </c>
-      <c r="J84" s="14">
-        <v>182.571</v>
-      </c>
-      <c r="K84" s="14">
-        <v>381</v>
-      </c>
-      <c r="L84" s="14">
-        <v>455</v>
-      </c>
-      <c r="M84" s="14">
-        <v>444</v>
-      </c>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" s="14">
-        <v>6.2939999999999996</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>3</v>
-      </c>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="14"/>
-      <c r="G85" s="14">
-        <v>50.076000000000001</v>
-      </c>
-      <c r="H85" s="14">
-        <v>174.749</v>
-      </c>
-      <c r="I85" s="14">
-        <v>16.385000000000002</v>
-      </c>
-      <c r="J85" s="14">
-        <v>65.694999999999993</v>
-      </c>
-      <c r="K85" s="14">
-        <v>35</v>
-      </c>
-      <c r="L85" s="14">
-        <v>54</v>
-      </c>
-      <c r="M85" s="14">
-        <v>115</v>
-      </c>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="14"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B86" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C86" s="14">
-        <v>1.7010000000000001</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>3</v>
-      </c>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="14"/>
       <c r="G86" s="14"/>
@@ -8513,126 +8543,6 @@
       <c r="K86" s="14"/>
       <c r="L86" s="14"/>
       <c r="M86" s="14"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B87" s="14">
-        <v>86.224999999999994</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="14"/>
-      <c r="K87" s="14"/>
-      <c r="L87" s="14"/>
-      <c r="M87" s="14"/>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B88" s="14">
-        <v>19.073</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
-      <c r="H88" s="14"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="14"/>
-      <c r="K88" s="14"/>
-      <c r="L88" s="14"/>
-      <c r="M88" s="14"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B89" s="14">
-        <v>1.7909999999999999</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="14"/>
-      <c r="M89" s="14"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B90" s="14">
-        <v>183</v>
-      </c>
-      <c r="C90" s="14">
-        <v>4.4820000000000002</v>
-      </c>
-      <c r="D90" s="14">
-        <v>2.7029999999999998</v>
-      </c>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
-      <c r="J90" s="14"/>
-      <c r="K90" s="14"/>
-      <c r="L90" s="14"/>
-      <c r="M90" s="14"/>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
-      <c r="I91" s="14"/>
-      <c r="J91" s="14"/>
-      <c r="K91" s="14"/>
-      <c r="L91" s="14"/>
-      <c r="M91" s="14"/>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B92" s="14"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14"/>
-      <c r="J92" s="14"/>
-      <c r="K92" s="14"/>
-      <c r="L92" s="14"/>
-      <c r="M92" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10585,7 +10495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3250EDC-943F-44FB-BA9C-BC28012A4183}">
   <dimension ref="A1:X93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
@@ -10599,31 +10509,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="69" t="s">
         <v>198</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
     </row>
     <row r="2" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="31"/>
@@ -10660,13 +10570,13 @@
       <c r="H3" s="32"/>
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="66" t="s">
         <v>196</v>
       </c>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="35"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="68"/>
       <c r="P3" s="32"/>
       <c r="Q3" s="32"/>
       <c r="R3" s="32"/>
@@ -10683,27 +10593,27 @@
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
-      <c r="G4" s="36"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
-      <c r="K4" s="53">
+      <c r="K4" s="48">
         <f>+B45</f>
         <v>2016</v>
       </c>
-      <c r="L4" s="54">
+      <c r="L4" s="49">
         <f>+C45</f>
         <v>2017</v>
       </c>
-      <c r="M4" s="54">
+      <c r="M4" s="49">
         <f>+D45</f>
         <v>2018</v>
       </c>
-      <c r="N4" s="54">
+      <c r="N4" s="49">
         <f>+E45</f>
         <v>2019</v>
       </c>
-      <c r="O4" s="55">
+      <c r="O4" s="50">
         <f>+F45</f>
         <v>2020</v>
       </c>
@@ -10718,44 +10628,44 @@
       <c r="X4" s="32"/>
     </row>
     <row r="5" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38">
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="35">
         <f>+B92</f>
         <v>-0.16264684947814087</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="36">
         <f>+C92</f>
         <v>-0.52878216538021661</v>
       </c>
-      <c r="M5" s="39">
+      <c r="M5" s="36">
         <f>+D92</f>
         <v>-0.215925248832013</v>
       </c>
-      <c r="N5" s="39">
+      <c r="N5" s="36">
         <f>+E92</f>
         <v>-0.11708717328901647</v>
       </c>
-      <c r="O5" s="40">
+      <c r="O5" s="37">
         <f>+F92</f>
         <v>3.8785151856017996E-2</v>
       </c>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="32"/>
@@ -10766,7 +10676,7 @@
       <c r="G6" s="32"/>
       <c r="H6" s="32"/>
       <c r="I6" s="32"/>
-      <c r="J6" s="41"/>
+      <c r="J6" s="38"/>
       <c r="K6" s="32"/>
       <c r="L6" s="32"/>
       <c r="M6" s="32"/>
@@ -10811,32 +10721,32 @@
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
       <c r="D8" s="32"/>
-      <c r="E8" s="33" t="str">
+      <c r="E8" s="66" t="str">
         <f>+A49</f>
         <v>Net Profit Ratio</v>
       </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="35"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="68"/>
       <c r="J8" s="32"/>
-      <c r="K8" s="33" t="str">
+      <c r="K8" s="66" t="str">
         <f>+A86</f>
         <v>Total Assets to Equity</v>
       </c>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="35"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="68"/>
       <c r="P8" s="32"/>
-      <c r="Q8" s="33" t="str">
+      <c r="Q8" s="66" t="str">
         <f>+A65</f>
         <v>Total Asset Turnover Ratio</v>
       </c>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="35"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="67"/>
+      <c r="U8" s="68"/>
       <c r="V8" s="32"/>
       <c r="W8" s="32"/>
       <c r="X8" s="32"/>
@@ -10845,65 +10755,65 @@
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
-      <c r="E9" s="53">
+      <c r="E9" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="F9" s="54">
+      <c r="F9" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G9" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="H9" s="54">
+      <c r="H9" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="I9" s="55">
+      <c r="I9" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="J9" s="32"/>
-      <c r="K9" s="53">
+      <c r="K9" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="L9" s="54">
+      <c r="L9" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="M9" s="54">
+      <c r="M9" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="N9" s="54">
+      <c r="N9" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="O9" s="55">
+      <c r="O9" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="P9" s="32"/>
-      <c r="Q9" s="53">
+      <c r="Q9" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="R9" s="54">
+      <c r="R9" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="S9" s="54">
+      <c r="S9" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="T9" s="54">
+      <c r="T9" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="U9" s="55">
+      <c r="U9" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
@@ -10915,65 +10825,65 @@
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
-      <c r="E10" s="38">
+      <c r="E10" s="35">
         <f>+B49</f>
         <v>-0.11043306040514665</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="36">
         <f>+C49</f>
         <v>-0.19054557750223641</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="36">
         <f>+D49</f>
         <v>-4.9531708680862964E-2</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="36">
         <f>+E49</f>
         <v>-3.1532264626902111E-2</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="37">
         <f>+F49</f>
         <v>2.7333840690005072E-2</v>
       </c>
       <c r="J10" s="32"/>
-      <c r="K10" s="38">
+      <c r="K10" s="35">
         <f>+B86</f>
         <v>4.7684621066962967</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="36">
         <f>+C86</f>
         <v>6.7627414247286328</v>
       </c>
-      <c r="M10" s="39">
+      <c r="M10" s="36">
         <f>+D86</f>
         <v>6.041031891123299</v>
       </c>
-      <c r="N10" s="39">
+      <c r="N10" s="36">
         <f>+E86</f>
         <v>5.1834113914488595</v>
       </c>
-      <c r="O10" s="40">
+      <c r="O10" s="37">
         <f>+F86</f>
         <v>2.3463667041619796</v>
       </c>
       <c r="P10" s="32"/>
-      <c r="Q10" s="56">
+      <c r="Q10" s="51">
         <f>+B65</f>
         <v>0.30886465435431826</v>
       </c>
-      <c r="R10" s="57">
+      <c r="R10" s="52">
         <f t="shared" ref="R10:U10" si="0">+C65</f>
         <v>0.4103506665347077</v>
       </c>
-      <c r="S10" s="57">
+      <c r="S10" s="52">
         <f t="shared" si="0"/>
         <v>0.72162071284465368</v>
       </c>
-      <c r="T10" s="57">
+      <c r="T10" s="52">
         <f t="shared" si="0"/>
         <v>0.71637179748753976</v>
       </c>
-      <c r="U10" s="58">
+      <c r="U10" s="53">
         <f t="shared" si="0"/>
         <v>0.60474035437600671</v>
       </c>
@@ -11007,206 +10917,206 @@
       <c r="X11" s="32"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="33" t="str">
+      <c r="B12" s="66" t="str">
         <f>+A88</f>
         <v>Capital Structure Impact</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
       <c r="G12" s="32"/>
-      <c r="H12" s="33" t="str">
+      <c r="H12" s="66" t="str">
         <f>+A51</f>
         <v>Tax Ratio</v>
       </c>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="35"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="68"/>
       <c r="M12" s="32"/>
-      <c r="N12" s="33" t="s">
+      <c r="N12" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="35"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="68"/>
       <c r="S12" s="32"/>
-      <c r="T12" s="33" t="s">
+      <c r="T12" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="U12" s="34"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
-      <c r="X12" s="35"/>
+      <c r="U12" s="67"/>
+      <c r="V12" s="67"/>
+      <c r="W12" s="67"/>
+      <c r="X12" s="68"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="53">
+      <c r="B13" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="G13" s="32"/>
-      <c r="H13" s="53">
+      <c r="H13" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="J13" s="54">
+      <c r="J13" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="K13" s="54">
+      <c r="K13" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="L13" s="55">
+      <c r="L13" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="M13" s="32"/>
-      <c r="N13" s="53">
+      <c r="N13" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="O13" s="54">
+      <c r="O13" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="P13" s="54">
+      <c r="P13" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="Q13" s="54">
+      <c r="Q13" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="R13" s="55">
+      <c r="R13" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="S13" s="32"/>
-      <c r="T13" s="53">
+      <c r="T13" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="U13" s="54">
+      <c r="U13" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="V13" s="54">
+      <c r="V13" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="W13" s="54">
+      <c r="W13" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="X13" s="55">
+      <c r="X13" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
     </row>
     <row r="14" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="38">
+      <c r="B14" s="35">
         <f>+B88</f>
         <v>1.1183924236521114</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="36">
         <f>+C88</f>
         <v>1.3535022051534049</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="36">
         <f>+D88</f>
         <v>2.5902061855670104</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="36">
         <f>+E88</f>
         <v>9.6376811594202891</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="37">
         <f>+F88</f>
         <v>0.5787362086258776</v>
       </c>
       <c r="G14" s="32"/>
-      <c r="H14" s="38">
+      <c r="H14" s="35">
         <f>+B51</f>
         <v>-3.5771516772336767E-2</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="36">
         <f>+C51</f>
         <v>-1.4280463116876533E-2</v>
       </c>
-      <c r="J14" s="39">
+      <c r="J14" s="36">
         <f>+D51</f>
         <v>-5.7711442786069649E-2</v>
       </c>
-      <c r="K14" s="39">
+      <c r="K14" s="36">
         <f>+E51</f>
         <v>-0.16541353383458646</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="37">
         <f>+F51</f>
         <v>0.2530329289428076</v>
       </c>
       <c r="M14" s="32"/>
-      <c r="N14" s="42">
+      <c r="N14" s="39">
         <f>+B77</f>
         <v>1.170012085996941</v>
       </c>
-      <c r="O14" s="43">
+      <c r="O14" s="40">
         <f t="shared" ref="O14:R14" si="1">+C77</f>
         <v>1.1726477388930185</v>
       </c>
-      <c r="P14" s="43">
+      <c r="P14" s="40">
         <f t="shared" si="1"/>
         <v>1.8941747572815535</v>
       </c>
-      <c r="Q14" s="43">
+      <c r="Q14" s="40">
         <f t="shared" si="1"/>
         <v>2.3641785302039247</v>
       </c>
-      <c r="R14" s="44">
+      <c r="R14" s="41">
         <f t="shared" si="1"/>
         <v>2.4739938809131559</v>
       </c>
       <c r="S14" s="32"/>
-      <c r="T14" s="42">
+      <c r="T14" s="39">
         <f>+B78</f>
         <v>9.9116211566643777</v>
       </c>
-      <c r="U14" s="43">
+      <c r="U14" s="40">
         <f t="shared" ref="U14:X14" si="2">+C78</f>
         <v>30.253972542118209</v>
       </c>
-      <c r="V14" s="43">
+      <c r="V14" s="40">
         <f t="shared" si="2"/>
         <v>32.665144596651444</v>
       </c>
-      <c r="W14" s="43">
+      <c r="W14" s="40">
         <f t="shared" si="2"/>
         <v>22.242533936651583</v>
       </c>
-      <c r="X14" s="44">
+      <c r="X14" s="41">
         <f t="shared" si="2"/>
         <v>-492.75</v>
       </c>
@@ -11240,13 +11150,13 @@
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
       <c r="D16" s="32"/>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="66" t="s">
         <v>161</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="35"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="68"/>
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
       <c r="L16" s="32"/>
@@ -11267,23 +11177,23 @@
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
       <c r="D17" s="32"/>
-      <c r="E17" s="53">
+      <c r="E17" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H17" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="I17" s="55">
+      <c r="I17" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
@@ -11307,23 +11217,23 @@
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
-      <c r="E18" s="38">
+      <c r="E18" s="35">
         <f>+B48</f>
         <v>-9.533248801594027E-2</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="36">
         <f>+C48</f>
         <v>-0.13879756446921956</v>
       </c>
-      <c r="G18" s="39">
+      <c r="G18" s="36">
         <f>+D48</f>
         <v>-1.8079306649270769E-2</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="36">
         <f>+E48</f>
         <v>-2.8073887216209618E-3</v>
       </c>
-      <c r="I18" s="40">
+      <c r="I18" s="37">
         <f>+F48</f>
         <v>6.3229325215626589E-2</v>
       </c>
@@ -11369,204 +11279,204 @@
       <c r="X19" s="32"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="66" t="s">
         <v>160</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
       <c r="G20" s="32"/>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="66" t="s">
         <v>184</v>
       </c>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="35"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="68"/>
       <c r="M20" s="32"/>
-      <c r="N20" s="33" t="s">
+      <c r="N20" s="66" t="s">
         <v>204</v>
       </c>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="35"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="68"/>
       <c r="S20" s="32"/>
-      <c r="T20" s="33" t="s">
+      <c r="T20" s="66" t="s">
         <v>171</v>
       </c>
-      <c r="U20" s="34"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="35"/>
+      <c r="U20" s="67"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="67"/>
+      <c r="X20" s="68"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="53">
+      <c r="B21" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="D21" s="54">
+      <c r="D21" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="F21" s="55">
+      <c r="F21" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="G21" s="32"/>
-      <c r="H21" s="53">
+      <c r="H21" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="I21" s="54">
+      <c r="I21" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="J21" s="54">
+      <c r="J21" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="K21" s="54">
+      <c r="K21" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="L21" s="55">
+      <c r="L21" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="M21" s="32"/>
-      <c r="N21" s="53">
+      <c r="N21" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="O21" s="54">
+      <c r="O21" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="P21" s="54">
+      <c r="P21" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="Q21" s="54">
+      <c r="Q21" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="R21" s="55">
+      <c r="R21" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="S21" s="32"/>
-      <c r="T21" s="53">
+      <c r="T21" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="U21" s="54">
+      <c r="U21" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="V21" s="54">
+      <c r="V21" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="W21" s="54">
+      <c r="W21" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="X21" s="55">
+      <c r="X21" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
     </row>
     <row r="22" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="38">
+      <c r="B22" s="35">
         <f>+B47</f>
         <v>0.22846097759299397</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="36">
         <f t="shared" ref="C22:F22" si="3">+C47</f>
         <v>0.18900706376042831</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="36">
         <f t="shared" si="3"/>
         <v>0.18834164298028983</v>
       </c>
-      <c r="E22" s="39">
+      <c r="E22" s="36">
         <f t="shared" si="3"/>
         <v>0.1655545609895028</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="37">
         <f t="shared" si="3"/>
         <v>0.2102359208523592</v>
       </c>
       <c r="G22" s="32"/>
-      <c r="H22" s="61">
+      <c r="H22" s="56">
         <f>+B54</f>
         <v>1432189</v>
       </c>
-      <c r="I22" s="62">
+      <c r="I22" s="57">
         <f t="shared" ref="I22:L22" si="4">+C54</f>
         <v>2476500</v>
       </c>
-      <c r="J22" s="62">
+      <c r="J22" s="57">
         <f t="shared" si="4"/>
         <v>2835000</v>
       </c>
-      <c r="K22" s="62">
+      <c r="K22" s="57">
         <f t="shared" si="4"/>
         <v>2646000</v>
       </c>
-      <c r="L22" s="63">
+      <c r="L22" s="58">
         <f t="shared" si="4"/>
         <v>3145000</v>
       </c>
       <c r="M22" s="32"/>
-      <c r="N22" s="42">
+      <c r="N22" s="39">
         <f>+B74</f>
         <v>2.9031639898276715</v>
       </c>
-      <c r="O22" s="43">
+      <c r="O22" s="40">
         <f t="shared" ref="O22:R22" si="5">+C74</f>
         <v>3.9896512917058886</v>
       </c>
-      <c r="P22" s="43">
+      <c r="P22" s="40">
         <f t="shared" si="5"/>
         <v>5.1157121879588843</v>
       </c>
-      <c r="Q22" s="43">
+      <c r="Q22" s="40">
         <f t="shared" si="5"/>
         <v>5.4386104481569877</v>
       </c>
-      <c r="R22" s="44">
+      <c r="R22" s="41">
         <f t="shared" si="5"/>
         <v>4.1160138820029744</v>
       </c>
       <c r="S22" s="32"/>
-      <c r="T22" s="42">
+      <c r="T22" s="39">
         <f>+B69</f>
         <v>2.6123313989089962</v>
       </c>
-      <c r="U22" s="43">
+      <c r="U22" s="40">
         <f t="shared" ref="U22:X22" si="6">+C69</f>
         <v>4.2129923213095255</v>
       </c>
-      <c r="V22" s="43">
+      <c r="V22" s="40">
         <f t="shared" si="6"/>
         <v>5.5955669771924192</v>
       </c>
-      <c r="W22" s="43">
+      <c r="W22" s="40">
         <f t="shared" si="6"/>
         <v>5.7739301801801801</v>
       </c>
-      <c r="X22" s="44">
+      <c r="X22" s="41">
         <f t="shared" si="6"/>
         <v>6.0731528895391369</v>
       </c>
@@ -11597,99 +11507,99 @@
       <c r="X23" s="32"/>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="68"/>
       <c r="G24" s="32"/>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="66" t="s">
         <v>185</v>
       </c>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="35"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="68"/>
       <c r="M24" s="32"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="33" t="s">
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="66" t="s">
         <v>205</v>
       </c>
-      <c r="R24" s="34"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="34"/>
-      <c r="U24" s="35"/>
+      <c r="R24" s="67"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="67"/>
+      <c r="U24" s="68"/>
       <c r="V24" s="32"/>
       <c r="W24" s="32"/>
       <c r="X24" s="32"/>
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="53">
+      <c r="B25" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="C25" s="54">
+      <c r="C25" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="D25" s="54">
+      <c r="D25" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="F25" s="55">
+      <c r="F25" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="G25" s="32"/>
-      <c r="H25" s="53">
+      <c r="H25" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="I25" s="54">
+      <c r="I25" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="J25" s="54">
+      <c r="J25" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="K25" s="54">
+      <c r="K25" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="L25" s="55">
+      <c r="L25" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="M25" s="32"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="53">
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="R25" s="54">
+      <c r="R25" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="S25" s="54">
+      <c r="S25" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="T25" s="54">
+      <c r="T25" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="U25" s="55">
+      <c r="U25" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
@@ -11698,68 +11608,68 @@
       <c r="X25" s="32"/>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="61">
+      <c r="B26" s="56">
         <f>+B56</f>
         <v>947099</v>
       </c>
-      <c r="C26" s="62">
+      <c r="C26" s="57">
         <f t="shared" ref="C26:F26" si="7">+C56</f>
         <v>1636003</v>
       </c>
-      <c r="D26" s="62">
+      <c r="D26" s="57">
         <f t="shared" si="7"/>
         <v>1901000</v>
       </c>
-      <c r="E26" s="62">
+      <c r="E26" s="57">
         <f t="shared" si="7"/>
         <v>2154000</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="58">
         <f t="shared" si="7"/>
         <v>2322000</v>
       </c>
       <c r="G26" s="32"/>
-      <c r="H26" s="61">
+      <c r="H26" s="56">
         <f>+B55</f>
         <v>834408</v>
       </c>
-      <c r="I26" s="62">
+      <c r="I26" s="57">
         <f t="shared" ref="I26:L26" si="8">+C55</f>
         <v>1378073</v>
       </c>
-      <c r="J26" s="62">
+      <c r="J26" s="57">
         <f t="shared" si="8"/>
         <v>1460000</v>
       </c>
-      <c r="K26" s="62">
+      <c r="K26" s="57">
         <f t="shared" si="8"/>
         <v>1343000</v>
       </c>
-      <c r="L26" s="63">
+      <c r="L26" s="58">
         <f t="shared" si="8"/>
         <v>1491000</v>
       </c>
       <c r="M26" s="32"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="42">
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="39">
         <f>+B72</f>
         <v>14.024329749850743</v>
       </c>
-      <c r="R26" s="43">
+      <c r="R26" s="40">
         <f t="shared" ref="R26:U26" si="9">+C72</f>
         <v>22.815647064986873</v>
       </c>
-      <c r="S26" s="43">
+      <c r="S26" s="40">
         <f t="shared" si="9"/>
         <v>22.614330874604846</v>
       </c>
-      <c r="T26" s="43">
+      <c r="T26" s="40">
         <f t="shared" si="9"/>
         <v>18.563444108761328</v>
       </c>
-      <c r="U26" s="44">
+      <c r="U26" s="41">
         <f t="shared" si="9"/>
         <v>16.721102863202546</v>
       </c>
@@ -11793,75 +11703,75 @@
       <c r="X27" s="32"/>
     </row>
     <row r="28" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="68"/>
       <c r="G28" s="32"/>
-      <c r="H28" s="33" t="s">
+      <c r="H28" s="66" t="s">
         <v>187</v>
       </c>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="35"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="68"/>
       <c r="M28" s="32"/>
       <c r="N28" s="32"/>
       <c r="O28" s="32"/>
       <c r="P28" s="32"/>
-      <c r="Q28" s="33" t="s">
+      <c r="Q28" s="66" t="s">
         <v>192</v>
       </c>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="35"/>
+      <c r="R28" s="67"/>
+      <c r="S28" s="67"/>
+      <c r="T28" s="67"/>
+      <c r="U28" s="68"/>
       <c r="V28" s="32"/>
       <c r="W28" s="32"/>
       <c r="X28" s="32"/>
     </row>
     <row r="29" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B29" s="53">
+      <c r="B29" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="C29" s="54">
+      <c r="C29" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="D29" s="54">
+      <c r="D29" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="E29" s="54">
+      <c r="E29" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="F29" s="55">
+      <c r="F29" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="G29" s="32"/>
-      <c r="H29" s="53">
+      <c r="H29" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="I29" s="54">
+      <c r="I29" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="J29" s="54">
+      <c r="J29" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="K29" s="54">
+      <c r="K29" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="L29" s="55">
+      <c r="L29" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
@@ -11869,23 +11779,23 @@
       <c r="N29" s="32"/>
       <c r="O29" s="32"/>
       <c r="P29" s="32"/>
-      <c r="Q29" s="53">
+      <c r="Q29" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="R29" s="54">
+      <c r="R29" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="S29" s="54">
+      <c r="S29" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="T29" s="54">
+      <c r="T29" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="U29" s="55">
+      <c r="U29" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
@@ -11894,44 +11804,44 @@
       <c r="X29" s="32"/>
     </row>
     <row r="30" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="61">
+      <c r="B30" s="56">
         <f>+B58</f>
         <v>194843</v>
       </c>
-      <c r="C30" s="62">
+      <c r="C30" s="57">
         <f t="shared" ref="C30:F30" si="10">+C58</f>
         <v>328472</v>
       </c>
-      <c r="D30" s="62">
+      <c r="D30" s="57">
         <f t="shared" si="10"/>
         <v>406000</v>
       </c>
-      <c r="E30" s="62">
+      <c r="E30" s="57">
         <f t="shared" si="10"/>
         <v>527000</v>
       </c>
-      <c r="F30" s="63">
+      <c r="F30" s="58">
         <f t="shared" si="10"/>
         <v>499000</v>
       </c>
       <c r="G30" s="32"/>
-      <c r="H30" s="61">
+      <c r="H30" s="56">
         <f>+B57</f>
         <v>334225</v>
       </c>
-      <c r="I30" s="62">
+      <c r="I30" s="57">
         <f t="shared" ref="I30:L30" si="11">+C57</f>
         <v>466760</v>
       </c>
-      <c r="J30" s="62">
+      <c r="J30" s="57">
         <f t="shared" si="11"/>
         <v>749000</v>
       </c>
-      <c r="K30" s="62">
+      <c r="K30" s="57">
         <f t="shared" si="11"/>
         <v>898000</v>
       </c>
-      <c r="L30" s="63">
+      <c r="L30" s="58">
         <f t="shared" si="11"/>
         <v>1734000</v>
       </c>
@@ -11939,23 +11849,23 @@
       <c r="N30" s="32"/>
       <c r="O30" s="32"/>
       <c r="P30" s="32"/>
-      <c r="Q30" s="42">
+      <c r="Q30" s="39">
         <f>+B79</f>
         <v>2.0629786020105998</v>
       </c>
-      <c r="R30" s="43">
+      <c r="R30" s="40">
         <f t="shared" ref="R30:U30" si="12">+C79</f>
         <v>3.4914047686490806</v>
       </c>
-      <c r="S30" s="43">
+      <c r="S30" s="40">
         <f t="shared" si="12"/>
         <v>5.8223005968529575</v>
       </c>
-      <c r="T30" s="43">
+      <c r="T30" s="40">
         <f t="shared" si="12"/>
         <v>3.9211869814932991</v>
       </c>
-      <c r="U30" s="44">
+      <c r="U30" s="41">
         <f t="shared" si="12"/>
         <v>1.6269087907552622</v>
       </c>
@@ -11989,21 +11899,21 @@
       <c r="X31" s="31"/>
     </row>
     <row r="32" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="66" t="s">
         <v>189</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="35"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="68"/>
       <c r="G32" s="31"/>
-      <c r="H32" s="33" t="s">
+      <c r="H32" s="66" t="s">
         <v>190</v>
       </c>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="35"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="68"/>
       <c r="M32" s="31"/>
       <c r="N32" s="31"/>
       <c r="O32" s="31"/>
@@ -12018,44 +11928,44 @@
       <c r="X32" s="31"/>
     </row>
     <row r="33" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="53">
+      <c r="B33" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="C33" s="54">
+      <c r="C33" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="D33" s="54">
+      <c r="D33" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="E33" s="54">
+      <c r="E33" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="F33" s="55">
+      <c r="F33" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="G33" s="31"/>
-      <c r="H33" s="53">
+      <c r="H33" s="48">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="I33" s="54">
+      <c r="I33" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="J33" s="54">
+      <c r="J33" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="K33" s="54">
+      <c r="K33" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="L33" s="55">
+      <c r="L33" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
@@ -12073,44 +11983,44 @@
       <c r="X33" s="31"/>
     </row>
     <row r="34" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="61">
+      <c r="B34" s="56">
         <f>+B59</f>
         <v>-198810</v>
       </c>
-      <c r="C34" s="62">
+      <c r="C34" s="57">
         <f t="shared" ref="C34:F34" si="13">+C59</f>
         <v>-471259</v>
       </c>
-      <c r="D34" s="62">
+      <c r="D34" s="57">
         <f t="shared" si="13"/>
         <v>-663000</v>
       </c>
-      <c r="E34" s="62">
+      <c r="E34" s="57">
         <f t="shared" si="13"/>
         <v>-685000</v>
       </c>
-      <c r="F34" s="63">
+      <c r="F34" s="58">
         <f t="shared" si="13"/>
         <v>-748000</v>
       </c>
       <c r="G34" s="31"/>
-      <c r="H34" s="61">
+      <c r="H34" s="56">
         <f>+B60</f>
         <v>0</v>
       </c>
-      <c r="I34" s="62">
+      <c r="I34" s="57">
         <f t="shared" ref="I34:L34" si="14">+C60</f>
         <v>0</v>
       </c>
-      <c r="J34" s="62">
+      <c r="J34" s="57">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="K34" s="62">
+      <c r="K34" s="57">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="L34" s="63">
+      <c r="L34" s="58">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -12178,27 +12088,27 @@
       <c r="X36" s="31"/>
     </row>
     <row r="37" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="35"/>
+      <c r="C37" s="67"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="68"/>
       <c r="J37" s="31"/>
-      <c r="K37" s="33" t="s">
+      <c r="K37" s="66" t="s">
         <v>200</v>
       </c>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="34"/>
-      <c r="P37" s="34"/>
-      <c r="Q37" s="34"/>
-      <c r="R37" s="35"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="67"/>
+      <c r="N37" s="67"/>
+      <c r="O37" s="67"/>
+      <c r="P37" s="67"/>
+      <c r="Q37" s="67"/>
+      <c r="R37" s="68"/>
       <c r="S37" s="31"/>
       <c r="T37" s="31"/>
       <c r="U37" s="31"/>
@@ -12207,50 +12117,50 @@
       <c r="X37" s="31"/>
     </row>
     <row r="38" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="46"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="32"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="54">
+      <c r="D38" s="38"/>
+      <c r="E38" s="49">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="F38" s="54">
+      <c r="F38" s="49">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="G38" s="54">
+      <c r="G38" s="49">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="H38" s="54">
+      <c r="H38" s="49">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="I38" s="55">
+      <c r="I38" s="50">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
       <c r="J38" s="31"/>
-      <c r="K38" s="46"/>
+      <c r="K38" s="43"/>
       <c r="L38" s="32"/>
       <c r="M38" s="32"/>
-      <c r="N38" s="68">
+      <c r="N38" s="63">
         <f>+$K$4</f>
         <v>2016</v>
       </c>
-      <c r="O38" s="68">
+      <c r="O38" s="63">
         <f>+$L$4</f>
         <v>2017</v>
       </c>
-      <c r="P38" s="68">
+      <c r="P38" s="63">
         <f>+$M$4</f>
         <v>2018</v>
       </c>
-      <c r="Q38" s="68">
+      <c r="Q38" s="63">
         <f>+$N$4</f>
         <v>2019</v>
       </c>
-      <c r="R38" s="69">
+      <c r="R38" s="64">
         <f>+$O$4</f>
         <v>2020</v>
       </c>
@@ -12262,54 +12172,54 @@
       <c r="X38" s="31"/>
     </row>
     <row r="39" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="64">
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="59">
         <f>+B85</f>
         <v>3.5241911746296113</v>
       </c>
-      <c r="F39" s="64">
+      <c r="F39" s="59">
         <f t="shared" ref="F39:I39" si="15">+C85</f>
         <v>5.433482439756804</v>
       </c>
-      <c r="G39" s="64">
+      <c r="G39" s="59">
         <f t="shared" si="15"/>
         <v>4.7586837294332724</v>
       </c>
-      <c r="H39" s="64">
+      <c r="H39" s="59">
         <f t="shared" si="15"/>
         <v>3.9581507780631515</v>
       </c>
-      <c r="I39" s="65">
+      <c r="I39" s="60">
         <f t="shared" si="15"/>
         <v>1.2786501687289089</v>
       </c>
       <c r="J39" s="31"/>
-      <c r="K39" s="47" t="s">
+      <c r="K39" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="L39" s="41"/>
-      <c r="M39" s="41"/>
-      <c r="N39" s="66">
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="61">
         <f>+B64</f>
         <v>1.0742733187975642</v>
       </c>
-      <c r="O39" s="66">
+      <c r="O39" s="61">
         <f t="shared" ref="O39:R39" si="16">+C64</f>
         <v>0.8561306219029613</v>
       </c>
-      <c r="P39" s="66">
+      <c r="P39" s="61">
         <f t="shared" si="16"/>
         <v>0.83128189732812974</v>
       </c>
-      <c r="Q39" s="66">
+      <c r="Q39" s="61">
         <f t="shared" si="16"/>
         <v>1.1346207931002157</v>
       </c>
-      <c r="R39" s="67">
+      <c r="R39" s="62">
         <f t="shared" si="16"/>
         <v>1.8751403705783267</v>
       </c>
@@ -12321,54 +12231,54 @@
       <c r="X39" s="31"/>
     </row>
     <row r="40" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="39">
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="36">
         <f>+B82</f>
         <v>1.4400143406851085</v>
       </c>
-      <c r="F40" s="39">
+      <c r="F40" s="36">
         <f t="shared" ref="F40:I40" si="17">+C82</f>
         <v>2.4101170053539542</v>
       </c>
-      <c r="G40" s="39">
+      <c r="G40" s="36">
         <f t="shared" si="17"/>
         <v>2.4318504976640258</v>
       </c>
-      <c r="H40" s="39">
+      <c r="H40" s="36">
         <f t="shared" si="17"/>
         <v>2.0273455204713704</v>
       </c>
-      <c r="I40" s="40">
+      <c r="I40" s="37">
         <f t="shared" si="17"/>
         <v>0.52589426321709787</v>
       </c>
       <c r="J40" s="31"/>
-      <c r="K40" s="48" t="s">
+      <c r="K40" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="59">
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="54">
         <f>+B63</f>
         <v>0.71946771969476597</v>
       </c>
-      <c r="O40" s="59">
+      <c r="O40" s="54">
         <f t="shared" ref="O40:R40" si="18">+C63</f>
         <v>0.56119455299055199</v>
       </c>
-      <c r="P40" s="59">
+      <c r="P40" s="54">
         <f t="shared" si="18"/>
         <v>0.519763834684279</v>
       </c>
-      <c r="Q40" s="59">
+      <c r="Q40" s="54">
         <f t="shared" si="18"/>
         <v>0.80163119902503044</v>
       </c>
-      <c r="R40" s="60">
+      <c r="R40" s="55">
         <f t="shared" si="18"/>
         <v>1.5873104997192589</v>
       </c>
@@ -12380,14 +12290,14 @@
       <c r="X40" s="31"/>
     </row>
     <row r="41" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
       <c r="L41" s="10"/>
@@ -12405,14 +12315,14 @@
       <c r="X41" s="10"/>
     </row>
     <row r="42" spans="1:24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="51" t="s">
+      <c r="A42" s="65" t="s">
         <v>202</v>
       </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
     </row>
     <row r="43" spans="1:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
@@ -13391,19 +13301,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="Q28:U28"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="K37:R37"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="N20:R20"/>
-    <mergeCell ref="T20:X20"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="H24:L24"/>
     <mergeCell ref="Q24:U24"/>
@@ -13416,6 +13313,19 @@
     <mergeCell ref="H12:L12"/>
     <mergeCell ref="N12:R12"/>
     <mergeCell ref="T12:X12"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="N20:R20"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="Q28:U28"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="K37:R37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>